<commit_message>
pas-12877: Partial Match UT SS
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/PartialMatch_UT_SS.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/PartialMatch_UT_SS.xlsx
@@ -29,7 +29,7 @@
     <author>Petrenko, Viktor (C)</author>
   </authors>
   <commentList>
-    <comment ref="AA2" authorId="0" shapeId="0">
+    <comment ref="Z2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>VIN</t>
   </si>
@@ -195,15 +195,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>STAT</t>
-  </si>
-  <si>
-    <t>CHOICE_TIER</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>8L V12</t>
   </si>
   <si>
@@ -213,12 +204,6 @@
     <t>VOLKSWAGEN</t>
   </si>
   <si>
-    <t>RT</t>
-  </si>
-  <si>
-    <t>7MSRP15H&amp;V</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -232,6 +217,9 @@
   </si>
   <si>
     <t>SEDAN</t>
+  </si>
+  <si>
+    <t>7PRTL15H&amp;V</t>
   </si>
 </sst>
 </file>
@@ -588,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A2:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,15 +598,14 @@
     <col min="23" max="23" width="22.33203125" customWidth="1"/>
     <col min="24" max="24" width="20.88671875" customWidth="1"/>
     <col min="25" max="25" width="34.6640625" customWidth="1"/>
-    <col min="26" max="26" width="5.88671875" customWidth="1"/>
-    <col min="27" max="27" width="16.33203125" customWidth="1"/>
-    <col min="28" max="29" width="13.6640625" customWidth="1"/>
-    <col min="35" max="35" width="19.88671875" customWidth="1"/>
-    <col min="36" max="36" width="21.88671875" customWidth="1"/>
-    <col min="38" max="38" width="20.88671875" customWidth="1"/>
+    <col min="26" max="26" width="16.33203125" customWidth="1"/>
+    <col min="27" max="27" width="13.6640625" customWidth="1"/>
+    <col min="33" max="33" width="19.88671875" customWidth="1"/>
+    <col min="34" max="34" width="21.88671875" customWidth="1"/>
+    <col min="36" max="36" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,66 +682,60 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3">
         <v>2018</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H2" s="3">
         <v>88888</v>
@@ -763,19 +744,19 @@
         <v>28</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O2" s="3">
         <v>12</v>
@@ -787,7 +768,7 @@
         <v>214</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="S2" s="3">
         <v>4</v>
@@ -810,43 +791,37 @@
       <c r="Y2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="3" t="s">
-        <v>51</v>
+      <c r="Z2" s="3">
+        <v>66</v>
       </c>
       <c r="AA2" s="3">
-        <v>66</v>
-      </c>
-      <c r="AB2" s="3">
         <v>55</v>
       </c>
+      <c r="AB2" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="AC2" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AD2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>20000101</v>
+      </c>
+      <c r="AH2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI2" s="3">
-        <v>20000101</v>
+      <c r="AI2" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL2" s="3" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>